<commit_message>
Added procedure notes to excel
</commit_message>
<xml_diff>
--- a/react-frontend/JsonForBuyerSeller.xlsx
+++ b/react-frontend/JsonForBuyerSeller.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://informatica-my.sharepoint.com/personal/dgaglani_informatica_com/Documents/DesktopFiles/sideprojects/sideprojects/react-frontend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{7BC6AA48-3428-40E4-89A4-D8DE010C4530}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B5DDB7A2-821C-46B2-9164-36C832E160B5}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="8_{7BC6AA48-3428-40E4-89A4-D8DE010C4530}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{636B761D-351B-49D7-86A6-EB47AB3267F1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{7C0BD582-EF6A-4AB0-8BC3-EDE756B78C10}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{7C0BD582-EF6A-4AB0-8BC3-EDE756B78C10}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Practice" sheetId="1" r:id="rId1"/>
+    <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>SamsungS9</t>
   </si>
@@ -57,6 +58,50 @@
   </si>
   <si>
     <t>Visitor from India</t>
+  </si>
+  <si>
+    <t>Deduced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Query: If I have to find what to buy in USA: I will query for buyer or seller as USA and …. </t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Answer procedure</t>
+  </si>
+  <si>
+    <t>What concrete questions do we want to answer, how to answer and how well does our data model fare in answering those</t>
+  </si>
+  <si>
+    <t>Spacial requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given a product (say Samsung s9) which country has the lowest and highest price for it </t>
+  </si>
+  <si>
+    <t>Given I am travelling to somewhere (say USA) from somewhere (say India) what are the items I should buy while going to there and coming back from there in order to generate maximum profit</t>
+  </si>
+  <si>
+    <t>PreCondition: No repeating buyerCountry and sellerCountry, individually repeatable but not together
+Given my data model looks like this {BuyInCountry: , SellInCountry: , profit:, product:} I will query by product=%Desired_product% and profit &gt; 0 and order by highest to lowest, I will make another query with product=%Desired_product% and profit &lt; 0 ordered by lowest to highest, switch the sign on profit, switch the buyer and seller and merge the lists.</t>
+  </si>
+  <si>
+    <t>25 Products * 20 Countries * 20 Countries - So given 4 GB of space I can get top 25 products for 20 countries</t>
+  </si>
+  <si>
+    <t>Given a country (say India) I want to find out what item I should buy here that will generate maximum profit for me and where should I sell it.</t>
+  </si>
+  <si>
+    <t>I will first visit the site when I am in India. I will select destination as USA and select 'seller' as my trader type, the system first makes a call with buyer as India and seller as US where profit &gt; 0 and arrange the list by descending order of profit, it then makes a call as Seller as india and Buyer as US and profit &lt; 0 and it arranges in decreasing order (highest negative to lowest negative), it then flips the sign and the buyer and seller (so buyer becomes India and seller becomes US)
+I will then visit the site from US where the process reverses</t>
+  </si>
+  <si>
+    <t>I will query on buyer as India or seller as India and for buyer as India call I will order by descending order in profit and for seller as India call I filter on profit &lt; 0, I will order by ascending order of profit (highest negative to lowest negative) and flip the sign and the buyer and seller</t>
+  </si>
+  <si>
+    <t>each entry comprising of {BuyInCountry: , SellInCountry: , profit:, product:} has 100 chars (400 Bytes) so 10 items for 4KB, 100 items for 40KB, 1000 items for 4MB, 10000 items for 40MB, 1 Lakh for 4 GB</t>
   </si>
 </sst>
 </file>
@@ -92,8 +137,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,17 +467,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA414B71-0CEB-4FEB-8A74-C3992D359567}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="49.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="48.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="66.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="63.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="62.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -472,8 +529,8 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4">
-        <v>20000</v>
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -489,11 +546,11 @@
       <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="D5">
-        <v>30000</v>
-      </c>
-      <c r="E5">
-        <v>10000</v>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -506,17 +563,22 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6">
-        <v>40000</v>
-      </c>
-      <c r="E6">
-        <v>20000</v>
-      </c>
-      <c r="F6">
-        <v>10000</v>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
       </c>
       <c r="G6">
         <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L8" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -563,60 +625,134 @@
         <v>India</v>
       </c>
     </row>
+    <row r="17" spans="12:14" x14ac:dyDescent="0.3">
+      <c r="L17" s="1"/>
+    </row>
     <row r="20" spans="12:14" x14ac:dyDescent="0.3">
       <c r="L20" t="str">
-        <f ca="1">_xlfn.CONCAT("{buyer:",OFFSET($C$2,ROW(C3)-ROW($C$2),0,1,1),",seller:",OFFSET($C$2,0,COLUMN(D3)-COLUMN($C$2),1,1),", diff:",D3,",product:", $C$2,"}")</f>
-        <v>{buyer:India,seller:India, diff:0,product:SamsungS9}</v>
+        <f ca="1">_xlfn.CONCAT("{buyInCountry:",OFFSET($C$2,ROW(C3)-ROW($C$2),0,1,1),",sellInCountry:",OFFSET($C$2,0,COLUMN(D3)-COLUMN($C$2),1,1),", profit:",D3,",product:", $C$2,"}")</f>
+        <v>{buyInCountry:India,sellInCountry:India, profit:0,product:SamsungS9}</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" ref="M20:N23" ca="1" si="0">_xlfn.CONCAT("{buyer:",OFFSET($C$2,ROW(D3)-ROW($C$2),0,1,1),",seller:",OFFSET($C$2,0,COLUMN(E3)-COLUMN($C$2),1,1),", diff:",E3,",product:", $C$2,"}")</f>
-        <v>{buyer:India,seller:USA, diff:-20000,product:SamsungS9}</v>
+        <f t="shared" ref="M20:N23" ca="1" si="0">_xlfn.CONCAT("{buyInCountry:",OFFSET($C$2,ROW(D3)-ROW($C$2),0,1,1),",sellInCountry:",OFFSET($C$2,0,COLUMN(E3)-COLUMN($C$2),1,1),", profit:",E3,",product:", $C$2,"}")</f>
+        <v>{buyInCountry:India,sellInCountry:USA, profit:-20000,product:SamsungS9}</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>{buyer:India,seller:Brajeel, diff:-30000,product:SamsungS9}</v>
+        <v>{buyInCountry:India,sellInCountry:Brajeel, profit:-30000,product:SamsungS9}</v>
       </c>
     </row>
     <row r="21" spans="12:14" x14ac:dyDescent="0.3">
       <c r="L21" t="str">
-        <f t="shared" ref="L21:L24" ca="1" si="1">_xlfn.CONCAT("{buyer:",OFFSET($C$2,ROW(C4)-ROW($C$2),0,1,1),",seller:",OFFSET($C$2,0,COLUMN(D4)-COLUMN($C$2),1,1),", diff:",D4,",product:", $C$2,"}")</f>
-        <v>{buyer:USA,seller:India, diff:20000,product:SamsungS9}</v>
+        <f t="shared" ref="L21:L23" ca="1" si="1">_xlfn.CONCAT("{buyInCountry:",OFFSET($C$2,ROW(C4)-ROW($C$2),0,1,1),",sellInCountry:",OFFSET($C$2,0,COLUMN(D4)-COLUMN($C$2),1,1),", profit:",D4,",product:", $C$2,"}")</f>
+        <v>{buyInCountry:USA,sellInCountry:India, profit:Deduced,product:SamsungS9}</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>{buyer:USA,seller:USA, diff:0,product:SamsungS9}</v>
+        <v>{buyInCountry:USA,sellInCountry:USA, profit:0,product:SamsungS9}</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>{buyer:USA,seller:Brajeel, diff:-10000,product:SamsungS9}</v>
+        <v>{buyInCountry:USA,sellInCountry:Brajeel, profit:-10000,product:SamsungS9}</v>
       </c>
     </row>
     <row r="22" spans="12:14" x14ac:dyDescent="0.3">
       <c r="L22" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>{buyer:Brajeel,seller:India, diff:30000,product:SamsungS9}</v>
+        <v>{buyInCountry:Brajeel,sellInCountry:India, profit:Deduced,product:SamsungS9}</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>{buyer:Brajeel,seller:USA, diff:10000,product:SamsungS9}</v>
+        <v>{buyInCountry:Brajeel,sellInCountry:USA, profit:Deduced,product:SamsungS9}</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>{buyer:Brajeel,seller:Brajeel, diff:0,product:SamsungS9}</v>
+        <v>{buyInCountry:Brajeel,sellInCountry:Brajeel, profit:0,product:SamsungS9}</v>
       </c>
     </row>
     <row r="23" spans="12:14" x14ac:dyDescent="0.3">
       <c r="L23" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>{buyer:Cheena,seller:India, diff:40000,product:SamsungS9}</v>
+        <v>{buyInCountry:Cheena,sellInCountry:India, profit:Deduced,product:SamsungS9}</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>{buyer:Cheena,seller:USA, diff:20000,product:SamsungS9}</v>
+        <v>{buyInCountry:Cheena,sellInCountry:USA, profit:Deduced,product:SamsungS9}</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>{buyer:Cheena,seller:Brajeel, diff:10000,product:SamsungS9}</v>
+        <v>{buyInCountry:Cheena,sellInCountry:Brajeel, profit:Deduced,product:SamsungS9}</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1004B4B8-CB00-4BEF-BCCC-BEEC149880AB}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="81.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>